<commit_message>
Datos edu hechos, a óscar le han hackeado el github
</commit_message>
<xml_diff>
--- a/excel/DatosEdu.xlsx
+++ b/excel/DatosEdu.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="462" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="32">
   <si>
     <t>Lugar de Partida</t>
   </si>
@@ -62,7 +62,7 @@
     <t>Habitual</t>
   </si>
   <si>
-    <t>Mañana</t>
+    <t>Manana</t>
   </si>
   <si>
     <t>Despejado</t>
@@ -74,13 +74,10 @@
     <t>Buena</t>
   </si>
   <si>
-    <t>EntreSemana</t>
+    <t>Laboral</t>
   </si>
   <si>
     <t>Carretera</t>
-  </si>
-  <si>
-    <t>Despejado </t>
   </si>
   <si>
     <t>Media Jornada</t>
@@ -89,7 +86,7 @@
     <t>Finde</t>
   </si>
   <si>
-    <t>Medio</t>
+    <t>Alto</t>
   </si>
   <si>
     <t>Nublado</t>
@@ -99,9 +96,6 @@
   </si>
   <si>
     <t>Tarde</t>
-  </si>
-  <si>
-    <t>Poco</t>
   </si>
   <si>
     <t>Tormentoso</t>
@@ -117,12 +111,6 @@
   </si>
   <si>
     <t>30</t>
-  </si>
-  <si>
-    <t>Laboral</t>
-  </si>
-  <si>
-    <t>Alto</t>
   </si>
 </sst>
 </file>
@@ -212,7 +200,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -257,10 +245,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -292,8 +276,8 @@
   </sheetPr>
   <dimension ref="A1:K142"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J56" activeCellId="0" sqref="J56:J136"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -303,12 +287,12 @@
     <col collapsed="false" hidden="false" max="4" min="3" style="1" width="10.5"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.6259259259259"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.5"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.8740740740741"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.8777777777778"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.5"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.2555555555556"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="8.6037037037037"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.33703703703704"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="2" width="10.5"/>
     <col collapsed="false" hidden="false" max="254" min="12" style="1" width="8.87037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="255" style="0" width="8.53333333333333"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -566,7 +550,7 @@
         <v>15</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>17</v>
@@ -601,7 +585,7 @@
         <v>15</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>17</v>
@@ -738,7 +722,7 @@
         <v>14</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>16</v>
@@ -750,7 +734,7 @@
         <v>18</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>20</v>
@@ -773,7 +757,7 @@
         <v>14</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>16</v>
@@ -785,7 +769,7 @@
         <v>18</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>20</v>
@@ -808,10 +792,10 @@
         <v>14</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>17</v>
@@ -820,7 +804,7 @@
         <v>18</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J16" s="8" t="s">
         <v>20</v>
@@ -843,10 +827,10 @@
         <v>14</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>17</v>
@@ -855,7 +839,7 @@
         <v>18</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J17" s="8" t="s">
         <v>20</v>
@@ -878,7 +862,7 @@
         <v>14</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>16</v>
@@ -890,7 +874,7 @@
         <v>18</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>20</v>
@@ -913,7 +897,7 @@
         <v>14</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>16</v>
@@ -925,7 +909,7 @@
         <v>18</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J19" s="8" t="s">
         <v>20</v>
@@ -948,7 +932,7 @@
         <v>14</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>16</v>
@@ -960,7 +944,7 @@
         <v>18</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J20" s="8" t="s">
         <v>20</v>
@@ -980,10 +964,10 @@
         <v>75</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>16</v>
@@ -995,7 +979,7 @@
         <v>18</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J21" s="8" t="s">
         <v>20</v>
@@ -1015,13 +999,13 @@
         <v>75</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>17</v>
@@ -1030,7 +1014,7 @@
         <v>18</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J22" s="8" t="s">
         <v>20</v>
@@ -1050,13 +1034,13 @@
         <v>75</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>17</v>
@@ -1065,7 +1049,7 @@
         <v>18</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J23" s="8" t="s">
         <v>20</v>
@@ -1085,13 +1069,13 @@
         <v>75</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>17</v>
@@ -1100,7 +1084,7 @@
         <v>18</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J24" s="8" t="s">
         <v>20</v>
@@ -1120,13 +1104,13 @@
         <v>75</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>17</v>
@@ -1135,7 +1119,7 @@
         <v>18</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J25" s="8" t="s">
         <v>20</v>
@@ -1155,13 +1139,13 @@
         <v>75</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>17</v>
@@ -1170,7 +1154,7 @@
         <v>18</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J26" s="8" t="s">
         <v>20</v>
@@ -1190,13 +1174,13 @@
         <v>75</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>17</v>
@@ -1205,7 +1189,7 @@
         <v>18</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J27" s="8" t="s">
         <v>20</v>
@@ -1225,13 +1209,13 @@
         <v>75</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>17</v>
@@ -1240,7 +1224,7 @@
         <v>18</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J28" s="8" t="s">
         <v>20</v>
@@ -1260,13 +1244,13 @@
         <v>75</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>17</v>
@@ -1275,7 +1259,7 @@
         <v>18</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J29" s="8" t="s">
         <v>20</v>
@@ -1295,13 +1279,13 @@
         <v>75</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>17</v>
@@ -1310,7 +1294,7 @@
         <v>18</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J30" s="8" t="s">
         <v>20</v>
@@ -1330,13 +1314,13 @@
         <v>75</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>17</v>
@@ -1345,7 +1329,7 @@
         <v>18</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J31" s="8" t="s">
         <v>20</v>
@@ -1365,13 +1349,13 @@
         <v>75</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>17</v>
@@ -1380,7 +1364,7 @@
         <v>18</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J32" s="8" t="s">
         <v>20</v>
@@ -1400,13 +1384,13 @@
         <v>75</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>17</v>
@@ -1415,7 +1399,7 @@
         <v>18</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J33" s="8" t="s">
         <v>20</v>
@@ -1435,13 +1419,13 @@
         <v>75</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>17</v>
@@ -1450,7 +1434,7 @@
         <v>18</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J34" s="8" t="s">
         <v>20</v>
@@ -1470,13 +1454,13 @@
         <v>75</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>17</v>
@@ -1485,7 +1469,7 @@
         <v>18</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J35" s="8" t="s">
         <v>20</v>
@@ -1505,13 +1489,13 @@
         <v>75</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>17</v>
@@ -1520,7 +1504,7 @@
         <v>18</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J36" s="8" t="s">
         <v>20</v>
@@ -1540,13 +1524,13 @@
         <v>75</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>17</v>
@@ -1555,7 +1539,7 @@
         <v>18</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J37" s="8" t="s">
         <v>20</v>
@@ -1575,13 +1559,13 @@
         <v>75</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>17</v>
@@ -1590,7 +1574,7 @@
         <v>18</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J38" s="8" t="s">
         <v>20</v>
@@ -1610,13 +1594,13 @@
         <v>75</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>17</v>
@@ -1625,7 +1609,7 @@
         <v>18</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J39" s="8" t="s">
         <v>20</v>
@@ -1645,13 +1629,13 @@
         <v>75</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>17</v>
@@ -1660,7 +1644,7 @@
         <v>18</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J40" s="8" t="s">
         <v>20</v>
@@ -1680,13 +1664,13 @@
         <v>75</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>17</v>
@@ -1695,7 +1679,7 @@
         <v>18</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J41" s="8" t="s">
         <v>20</v>
@@ -1715,14 +1699,14 @@
         <v>75</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E42" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F42" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F42" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="G42" s="4" t="s">
         <v>17</v>
       </c>
@@ -1730,7 +1714,7 @@
         <v>18</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J42" s="8" t="s">
         <v>20</v>
@@ -1750,14 +1734,14 @@
         <v>75</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E43" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F43" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F43" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="G43" s="4" t="s">
         <v>17</v>
       </c>
@@ -1765,7 +1749,7 @@
         <v>18</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J43" s="8" t="s">
         <v>20</v>
@@ -1785,13 +1769,13 @@
         <v>75</v>
       </c>
       <c r="D44" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E44" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="F44" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>17</v>
@@ -1800,7 +1784,7 @@
         <v>18</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J44" s="8" t="s">
         <v>20</v>
@@ -1820,13 +1804,13 @@
         <v>75</v>
       </c>
       <c r="D45" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E45" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="F45" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>17</v>
@@ -1835,7 +1819,7 @@
         <v>18</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J45" s="8" t="s">
         <v>20</v>
@@ -1855,13 +1839,13 @@
         <v>75</v>
       </c>
       <c r="D46" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E46" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="F46" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>17</v>
@@ -1870,7 +1854,7 @@
         <v>18</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J46" s="8" t="s">
         <v>20</v>
@@ -1890,13 +1874,13 @@
         <v>75</v>
       </c>
       <c r="D47" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E47" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E47" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="F47" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>17</v>
@@ -1905,7 +1889,7 @@
         <v>18</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J47" s="8" t="s">
         <v>20</v>
@@ -1925,13 +1909,13 @@
         <v>75</v>
       </c>
       <c r="D48" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E48" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E48" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="F48" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>17</v>
@@ -1940,7 +1924,7 @@
         <v>18</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J48" s="8" t="s">
         <v>20</v>
@@ -1960,13 +1944,13 @@
         <v>75</v>
       </c>
       <c r="D49" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E49" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E49" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="F49" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>17</v>
@@ -1975,7 +1959,7 @@
         <v>18</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J49" s="8" t="s">
         <v>20</v>
@@ -1995,13 +1979,13 @@
         <v>75</v>
       </c>
       <c r="D50" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E50" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E50" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="F50" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>17</v>
@@ -2010,7 +1994,7 @@
         <v>18</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J50" s="8" t="s">
         <v>20</v>
@@ -2030,13 +2014,13 @@
         <v>75</v>
       </c>
       <c r="D51" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E51" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E51" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="F51" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>17</v>
@@ -2045,7 +2029,7 @@
         <v>18</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J51" s="8" t="s">
         <v>20</v>
@@ -2065,13 +2049,13 @@
         <v>75</v>
       </c>
       <c r="D52" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E52" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E52" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="F52" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>17</v>
@@ -2080,7 +2064,7 @@
         <v>18</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J52" s="8" t="s">
         <v>20</v>
@@ -2100,13 +2084,13 @@
         <v>75</v>
       </c>
       <c r="D53" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E53" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E53" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="F53" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>17</v>
@@ -2115,7 +2099,7 @@
         <v>18</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J53" s="8" t="s">
         <v>20</v>
@@ -2135,13 +2119,13 @@
         <v>75</v>
       </c>
       <c r="D54" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E54" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="F54" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>17</v>
@@ -2150,7 +2134,7 @@
         <v>18</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J54" s="8" t="s">
         <v>20</v>
@@ -2174,13 +2158,13 @@
     </row>
     <row r="56" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>14</v>
@@ -2198,19 +2182,21 @@
         <v>18</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J56" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K56" s="5"/>
+      <c r="K56" s="5" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C57" s="5" t="n">
         <v>30</v>
@@ -2231,22 +2217,24 @@
         <v>18</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J57" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K57" s="5"/>
+      <c r="K57" s="5" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>14</v>
@@ -2264,22 +2252,24 @@
         <v>18</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J58" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K58" s="5"/>
+      <c r="K58" s="5" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>14</v>
@@ -2297,22 +2287,24 @@
         <v>18</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J59" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K59" s="5"/>
+      <c r="K59" s="5" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>14</v>
@@ -2330,22 +2322,24 @@
         <v>18</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J60" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K60" s="5"/>
+      <c r="K60" s="5" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>14</v>
@@ -2363,22 +2357,24 @@
         <v>18</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J61" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K61" s="5"/>
+      <c r="K61" s="5" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>14</v>
@@ -2396,22 +2392,24 @@
         <v>18</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J62" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K62" s="5"/>
+      <c r="K62" s="5" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>14</v>
@@ -2429,22 +2427,24 @@
         <v>18</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J63" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K63" s="5"/>
+      <c r="K63" s="5" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>14</v>
@@ -2462,22 +2462,24 @@
         <v>18</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J64" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K64" s="5"/>
+      <c r="K64" s="5" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>14</v>
@@ -2495,28 +2497,30 @@
         <v>18</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J65" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K65" s="5"/>
+      <c r="K65" s="5" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F66" s="4" t="s">
         <v>16</v>
@@ -2528,19 +2532,21 @@
         <v>18</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J66" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K66" s="5"/>
+      <c r="K66" s="5" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C67" s="5" t="n">
         <v>30</v>
@@ -2549,7 +2555,7 @@
         <v>14</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F67" s="4" t="s">
         <v>16</v>
@@ -2561,19 +2567,21 @@
         <v>18</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J67" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K67" s="5"/>
+      <c r="K67" s="5" t="n">
+        <v>32</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C68" s="5" t="n">
         <v>30</v>
@@ -2582,7 +2590,7 @@
         <v>14</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F68" s="4" t="s">
         <v>16</v>
@@ -2594,19 +2602,21 @@
         <v>18</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J68" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K68" s="5"/>
+      <c r="K68" s="5" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C69" s="5" t="n">
         <v>30</v>
@@ -2615,7 +2625,7 @@
         <v>14</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F69" s="4" t="s">
         <v>16</v>
@@ -2627,19 +2637,21 @@
         <v>18</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J69" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K69" s="5"/>
+      <c r="K69" s="5" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C70" s="5" t="n">
         <v>30</v>
@@ -2648,7 +2660,7 @@
         <v>14</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F70" s="4" t="s">
         <v>16</v>
@@ -2660,19 +2672,21 @@
         <v>18</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J70" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K70" s="5"/>
+      <c r="K70" s="5" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C71" s="5" t="n">
         <v>30</v>
@@ -2681,7 +2695,7 @@
         <v>14</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F71" s="4" t="s">
         <v>16</v>
@@ -2693,19 +2707,21 @@
         <v>18</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J71" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K71" s="5"/>
+      <c r="K71" s="5" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C72" s="5" t="n">
         <v>30</v>
@@ -2714,7 +2730,7 @@
         <v>14</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F72" s="4" t="s">
         <v>16</v>
@@ -2726,28 +2742,30 @@
         <v>18</v>
       </c>
       <c r="I72" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J72" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K72" s="5"/>
+      <c r="K72" s="5" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F73" s="4" t="s">
         <v>16</v>
@@ -2759,28 +2777,30 @@
         <v>18</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J73" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K73" s="5"/>
+      <c r="K73" s="5" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F74" s="4" t="s">
         <v>16</v>
@@ -2792,28 +2812,30 @@
         <v>18</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J74" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K74" s="5"/>
+      <c r="K74" s="5" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F75" s="4" t="s">
         <v>16</v>
@@ -2825,31 +2847,33 @@
         <v>18</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J75" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K75" s="5"/>
+      <c r="K75" s="5" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>17</v>
@@ -2858,31 +2882,33 @@
         <v>18</v>
       </c>
       <c r="I76" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J76" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K76" s="5"/>
+      <c r="K76" s="5" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>17</v>
@@ -2891,64 +2917,68 @@
         <v>18</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J77" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K77" s="5"/>
+      <c r="K77" s="5" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C78" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H78" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I78" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J78" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K78" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="D78" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E78" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F78" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G78" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H78" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I78" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J78" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K78" s="5"/>
     </row>
     <row r="79" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G79" s="4" t="s">
         <v>17</v>
@@ -2957,31 +2987,33 @@
         <v>18</v>
       </c>
       <c r="I79" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J79" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K79" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="J79" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K79" s="5"/>
     </row>
     <row r="80" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G80" s="4" t="s">
         <v>17</v>
@@ -2990,19 +3022,21 @@
         <v>18</v>
       </c>
       <c r="I80" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J80" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K80" s="5"/>
+      <c r="K80" s="5" t="n">
+        <v>38</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C81" s="5" t="n">
         <v>30</v>
@@ -3011,10 +3045,10 @@
         <v>14</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G81" s="4" t="s">
         <v>17</v>
@@ -3023,31 +3057,33 @@
         <v>18</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J81" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K81" s="5"/>
+      <c r="K81" s="5" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G82" s="4" t="s">
         <v>17</v>
@@ -3056,31 +3092,33 @@
         <v>18</v>
       </c>
       <c r="I82" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J82" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K82" s="5"/>
+      <c r="K82" s="5" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G83" s="4" t="s">
         <v>17</v>
@@ -3089,64 +3127,68 @@
         <v>18</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J83" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K83" s="5"/>
+      <c r="K83" s="5" t="n">
+        <v>36</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D84" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F84" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G84" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I84" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J84" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K84" s="5" t="n">
         <v>25</v>
       </c>
-      <c r="G84" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H84" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I84" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J84" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K84" s="5"/>
     </row>
     <row r="85" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G85" s="4" t="s">
         <v>17</v>
@@ -3155,31 +3197,33 @@
         <v>18</v>
       </c>
       <c r="I85" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J85" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K85" s="5"/>
+      <c r="K85" s="5" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G86" s="4" t="s">
         <v>17</v>
@@ -3188,31 +3232,33 @@
         <v>18</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J86" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K86" s="5"/>
+      <c r="K86" s="5" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G87" s="4" t="s">
         <v>17</v>
@@ -3221,19 +3267,21 @@
         <v>18</v>
       </c>
       <c r="I87" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J87" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K87" s="5"/>
+      <c r="K87" s="5" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C88" s="5" t="n">
         <v>30</v>
@@ -3242,10 +3290,10 @@
         <v>14</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G88" s="4" t="s">
         <v>17</v>
@@ -3254,64 +3302,68 @@
         <v>18</v>
       </c>
       <c r="I88" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J88" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K88" s="5"/>
+      <c r="K88" s="5" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="89" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F89" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I89" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J89" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K89" s="5" t="n">
         <v>25</v>
       </c>
-      <c r="G89" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H89" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I89" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J89" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K89" s="5"/>
     </row>
     <row r="90" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G90" s="4" t="s">
         <v>17</v>
@@ -3320,19 +3372,21 @@
         <v>18</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J90" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K90" s="5"/>
+      <c r="K90" s="5" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C91" s="5" t="n">
         <v>30</v>
@@ -3341,10 +3395,10 @@
         <v>14</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G91" s="4" t="s">
         <v>17</v>
@@ -3353,31 +3407,33 @@
         <v>18</v>
       </c>
       <c r="I91" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J91" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K91" s="5"/>
+      <c r="K91" s="5" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="92" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D92" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G92" s="4" t="s">
         <v>17</v>
@@ -3386,31 +3442,33 @@
         <v>18</v>
       </c>
       <c r="I92" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J92" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K92" s="5"/>
+      <c r="K92" s="5" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G93" s="4" t="s">
         <v>17</v>
@@ -3419,97 +3477,103 @@
         <v>18</v>
       </c>
       <c r="I93" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J93" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K93" s="5"/>
+      <c r="K93" s="5" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B94" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G94" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I94" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J94" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K94" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="C94" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D94" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E94" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F94" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G94" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H94" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I94" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J94" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K94" s="5"/>
     </row>
     <row r="95" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C95" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G95" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H95" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I95" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J95" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K95" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="D95" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E95" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F95" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G95" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H95" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I95" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J95" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K95" s="5"/>
     </row>
     <row r="96" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D96" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G96" s="4" t="s">
         <v>17</v>
@@ -3518,28 +3582,30 @@
         <v>18</v>
       </c>
       <c r="I96" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J96" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K96" s="5"/>
+      <c r="K96" s="5" t="n">
+        <v>34</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D97" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F97" s="4" t="s">
         <v>16</v>
@@ -3551,28 +3617,30 @@
         <v>18</v>
       </c>
       <c r="I97" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J97" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K97" s="5"/>
+      <c r="K97" s="5" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F98" s="4" t="s">
         <v>16</v>
@@ -3584,19 +3652,21 @@
         <v>18</v>
       </c>
       <c r="I98" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J98" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K98" s="5"/>
+      <c r="K98" s="5" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C99" s="5" t="n">
         <v>30</v>
@@ -3605,7 +3675,7 @@
         <v>14</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F99" s="4" t="s">
         <v>16</v>
@@ -3617,28 +3687,30 @@
         <v>18</v>
       </c>
       <c r="I99" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J99" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K99" s="5"/>
+      <c r="K99" s="5" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F100" s="4" t="s">
         <v>16</v>
@@ -3650,28 +3722,30 @@
         <v>18</v>
       </c>
       <c r="I100" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J100" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K100" s="5"/>
+      <c r="K100" s="5" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D101" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F101" s="4" t="s">
         <v>16</v>
@@ -3683,25 +3757,27 @@
         <v>18</v>
       </c>
       <c r="I101" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J101" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K101" s="5"/>
+      <c r="K101" s="5" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="102" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E102" s="4" t="s">
         <v>15</v>
@@ -3716,25 +3792,27 @@
         <v>18</v>
       </c>
       <c r="I102" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J102" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K102" s="5"/>
+      <c r="K102" s="5" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="103" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E103" s="4" t="s">
         <v>15</v>
@@ -3749,25 +3827,27 @@
         <v>18</v>
       </c>
       <c r="I103" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J103" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K103" s="5"/>
+      <c r="K103" s="5" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="104" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E104" s="4" t="s">
         <v>15</v>
@@ -3782,31 +3862,33 @@
         <v>18</v>
       </c>
       <c r="I104" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J104" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K104" s="5"/>
+      <c r="K104" s="5" t="n">
+        <v>34</v>
+      </c>
     </row>
     <row r="105" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E105" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G105" s="4" t="s">
         <v>17</v>
@@ -3815,31 +3897,33 @@
         <v>18</v>
       </c>
       <c r="I105" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J105" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K105" s="5"/>
+      <c r="K105" s="5" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="106" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E106" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G106" s="4" t="s">
         <v>17</v>
@@ -3848,31 +3932,33 @@
         <v>18</v>
       </c>
       <c r="I106" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J106" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K106" s="5"/>
+      <c r="K106" s="5" t="n">
+        <v>38</v>
+      </c>
     </row>
     <row r="107" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E107" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G107" s="4" t="s">
         <v>17</v>
@@ -3881,31 +3967,33 @@
         <v>18</v>
       </c>
       <c r="I107" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J107" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K107" s="5"/>
+      <c r="K107" s="5" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="108" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E108" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F108" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G108" s="4" t="s">
         <v>17</v>
@@ -3914,31 +4002,33 @@
         <v>18</v>
       </c>
       <c r="I108" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J108" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K108" s="5"/>
+      <c r="K108" s="5" t="n">
+        <v>45</v>
+      </c>
     </row>
     <row r="109" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F109" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G109" s="4" t="s">
         <v>17</v>
@@ -3947,31 +4037,33 @@
         <v>18</v>
       </c>
       <c r="I109" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J109" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K109" s="5"/>
+      <c r="K109" s="5" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="110" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E110" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F110" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G110" s="4" t="s">
         <v>17</v>
@@ -3980,97 +4072,103 @@
         <v>18</v>
       </c>
       <c r="I110" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J110" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K110" s="5"/>
+      <c r="K110" s="5" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="111" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B111" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D111" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E111" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F111" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G111" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H111" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I111" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J111" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K111" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="C111" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D111" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E111" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F111" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G111" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H111" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I111" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J111" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K111" s="5"/>
     </row>
     <row r="112" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C112" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D112" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E112" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F112" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G112" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H112" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I112" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J112" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K112" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="D112" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E112" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F112" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G112" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H112" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I112" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J112" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K112" s="5"/>
     </row>
     <row r="113" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E113" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F113" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G113" s="4" t="s">
         <v>17</v>
@@ -4079,31 +4177,33 @@
         <v>18</v>
       </c>
       <c r="I113" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J113" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K113" s="5"/>
+      <c r="K113" s="5" t="n">
+        <v>38</v>
+      </c>
     </row>
     <row r="114" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E114" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F114" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G114" s="4" t="s">
         <v>17</v>
@@ -4112,31 +4212,33 @@
         <v>18</v>
       </c>
       <c r="I114" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J114" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K114" s="5"/>
+      <c r="K114" s="5" t="n">
+        <v>42</v>
+      </c>
     </row>
     <row r="115" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C115" s="5" t="n">
         <v>30</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E115" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G115" s="4" t="s">
         <v>17</v>
@@ -4145,31 +4247,33 @@
         <v>18</v>
       </c>
       <c r="I115" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J115" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K115" s="5"/>
+      <c r="K115" s="5" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="116" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C116" s="5" t="n">
         <v>30</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E116" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F116" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G116" s="4" t="s">
         <v>17</v>
@@ -4178,31 +4282,33 @@
         <v>18</v>
       </c>
       <c r="I116" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J116" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K116" s="5"/>
+      <c r="K116" s="5" t="n">
+        <v>42</v>
+      </c>
     </row>
     <row r="117" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C117" s="5" t="n">
         <v>30</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E117" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G117" s="4" t="s">
         <v>17</v>
@@ -4211,31 +4317,33 @@
         <v>18</v>
       </c>
       <c r="I117" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J117" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K117" s="5"/>
+      <c r="K117" s="5" t="n">
+        <v>44</v>
+      </c>
     </row>
     <row r="118" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C118" s="5" t="n">
         <v>30</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E118" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F118" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G118" s="4" t="s">
         <v>17</v>
@@ -4244,31 +4352,33 @@
         <v>18</v>
       </c>
       <c r="I118" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J118" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K118" s="5"/>
+      <c r="K118" s="5" t="n">
+        <v>45</v>
+      </c>
     </row>
     <row r="119" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C119" s="5" t="n">
         <v>30</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E119" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F119" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G119" s="4" t="s">
         <v>17</v>
@@ -4277,31 +4387,33 @@
         <v>18</v>
       </c>
       <c r="I119" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J119" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K119" s="5"/>
+      <c r="K119" s="5" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="120" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C120" s="5" t="n">
         <v>30</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E120" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F120" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G120" s="4" t="s">
         <v>17</v>
@@ -4310,31 +4422,33 @@
         <v>18</v>
       </c>
       <c r="I120" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J120" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K120" s="5"/>
+      <c r="K120" s="5" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="121" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C121" s="5" t="n">
         <v>30</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E121" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F121" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G121" s="4" t="s">
         <v>17</v>
@@ -4343,32 +4457,34 @@
         <v>18</v>
       </c>
       <c r="I121" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J121" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K121" s="5"/>
+      <c r="K121" s="5" t="n">
+        <v>48</v>
+      </c>
     </row>
     <row r="122" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C122" s="5" t="n">
         <v>30</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E122" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F122" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F122" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="G122" s="4" t="s">
         <v>17</v>
       </c>
@@ -4376,31 +4492,33 @@
         <v>18</v>
       </c>
       <c r="I122" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J122" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K122" s="5"/>
+      <c r="K122" s="5" t="n">
+        <v>43</v>
+      </c>
     </row>
     <row r="123" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C123" s="5" t="n">
         <v>30</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E123" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F123" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G123" s="4" t="s">
         <v>17</v>
@@ -4409,64 +4527,68 @@
         <v>18</v>
       </c>
       <c r="I123" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J123" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K123" s="5"/>
+      <c r="K123" s="5" t="n">
+        <v>38</v>
+      </c>
     </row>
     <row r="124" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C124" s="5" t="n">
         <v>30</v>
       </c>
       <c r="D124" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E124" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F124" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G124" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H124" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I124" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J124" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K124" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="E124" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F124" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G124" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H124" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I124" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J124" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K124" s="5"/>
     </row>
     <row r="125" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C125" s="5" t="n">
         <v>30</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E125" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F125" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G125" s="4" t="s">
         <v>17</v>
@@ -4475,31 +4597,33 @@
         <v>18</v>
       </c>
       <c r="I125" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J125" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K125" s="5"/>
+      <c r="K125" s="5" t="n">
+        <v>38</v>
+      </c>
     </row>
     <row r="126" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C126" s="5" t="n">
         <v>30</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E126" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F126" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G126" s="4" t="s">
         <v>17</v>
@@ -4508,31 +4632,33 @@
         <v>18</v>
       </c>
       <c r="I126" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J126" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K126" s="5"/>
+      <c r="K126" s="5" t="n">
+        <v>38</v>
+      </c>
     </row>
     <row r="127" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C127" s="5" t="n">
         <v>30</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E127" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F127" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G127" s="4" t="s">
         <v>17</v>
@@ -4541,31 +4667,33 @@
         <v>18</v>
       </c>
       <c r="I127" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J127" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K127" s="5"/>
+      <c r="K127" s="5" t="n">
+        <v>36</v>
+      </c>
     </row>
     <row r="128" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C128" s="5" t="n">
         <v>30</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E128" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F128" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G128" s="4" t="s">
         <v>17</v>
@@ -4574,31 +4702,33 @@
         <v>18</v>
       </c>
       <c r="I128" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J128" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K128" s="5"/>
+      <c r="K128" s="5" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="129" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C129" s="5" t="n">
         <v>30</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E129" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F129" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G129" s="4" t="s">
         <v>17</v>
@@ -4607,64 +4737,68 @@
         <v>18</v>
       </c>
       <c r="I129" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J129" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K129" s="5"/>
+      <c r="K129" s="5" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="130" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B130" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C130" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="D130" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E130" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F130" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G130" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H130" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I130" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J130" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K130" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="C130" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="D130" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E130" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F130" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G130" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H130" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I130" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J130" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K130" s="5"/>
     </row>
     <row r="131" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C131" s="5" t="n">
         <v>30</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E131" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F131" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G131" s="4" t="s">
         <v>17</v>
@@ -4673,64 +4807,68 @@
         <v>18</v>
       </c>
       <c r="I131" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J131" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K131" s="5"/>
+      <c r="K131" s="5" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="132" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C132" s="5" t="n">
         <v>30</v>
       </c>
       <c r="D132" s="4" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="E132" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F132" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G132" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H132" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I132" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J132" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K132" s="5" t="n">
         <v>25</v>
       </c>
-      <c r="G132" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H132" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I132" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J132" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K132" s="5"/>
     </row>
     <row r="133" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C133" s="5" t="n">
         <v>30</v>
       </c>
       <c r="D133" s="4" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="E133" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F133" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G133" s="4" t="s">
         <v>17</v>
@@ -4739,31 +4877,33 @@
         <v>18</v>
       </c>
       <c r="I133" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J133" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K133" s="5"/>
+      <c r="K133" s="5" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="134" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C134" s="9" t="n">
         <v>30</v>
       </c>
       <c r="D134" s="4" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="E134" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F134" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G134" s="4" t="s">
         <v>17</v>
@@ -4772,64 +4912,68 @@
         <v>18</v>
       </c>
       <c r="I134" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J134" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K134" s="9"/>
+      <c r="K134" s="9" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="135" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C135" s="9" t="n">
         <v>30</v>
       </c>
       <c r="D135" s="4" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="E135" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F135" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G135" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H135" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I135" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J135" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K135" s="9" t="n">
         <v>25</v>
       </c>
-      <c r="G135" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H135" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I135" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J135" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K135" s="9"/>
     </row>
     <row r="136" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C136" s="10" t="n">
         <v>30</v>
       </c>
       <c r="D136" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E136" s="11" t="s">
-        <v>30</v>
+        <v>14</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="F136" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G136" s="4" t="s">
         <v>17</v>
@@ -4838,89 +4982,91 @@
         <v>18</v>
       </c>
       <c r="I136" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J136" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K136" s="9"/>
+      <c r="K136" s="9" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="137" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A137" s="12"/>
-      <c r="B137" s="12"/>
+      <c r="A137" s="11"/>
+      <c r="B137" s="11"/>
       <c r="C137" s="10"/>
-      <c r="D137" s="12"/>
+      <c r="D137" s="11"/>
       <c r="E137" s="0"/>
-      <c r="F137" s="12"/>
-      <c r="G137" s="12"/>
-      <c r="H137" s="13"/>
-      <c r="I137" s="13"/>
-      <c r="J137" s="14"/>
+      <c r="F137" s="11"/>
+      <c r="G137" s="11"/>
+      <c r="H137" s="12"/>
+      <c r="I137" s="12"/>
+      <c r="J137" s="13"/>
       <c r="K137" s="10"/>
     </row>
     <row r="138" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A138" s="12"/>
-      <c r="B138" s="12"/>
+      <c r="A138" s="11"/>
+      <c r="B138" s="11"/>
       <c r="C138" s="10"/>
-      <c r="D138" s="12"/>
+      <c r="D138" s="11"/>
       <c r="E138" s="0"/>
-      <c r="F138" s="12"/>
-      <c r="G138" s="12"/>
-      <c r="H138" s="13"/>
-      <c r="I138" s="13"/>
-      <c r="J138" s="14"/>
+      <c r="F138" s="11"/>
+      <c r="G138" s="11"/>
+      <c r="H138" s="12"/>
+      <c r="I138" s="12"/>
+      <c r="J138" s="13"/>
       <c r="K138" s="10"/>
     </row>
     <row r="139" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A139" s="12"/>
-      <c r="B139" s="12"/>
+      <c r="A139" s="11"/>
+      <c r="B139" s="11"/>
       <c r="C139" s="10"/>
-      <c r="D139" s="12"/>
+      <c r="D139" s="11"/>
       <c r="E139" s="0"/>
-      <c r="F139" s="12"/>
-      <c r="G139" s="12"/>
-      <c r="H139" s="13"/>
-      <c r="I139" s="13"/>
-      <c r="J139" s="14"/>
+      <c r="F139" s="11"/>
+      <c r="G139" s="11"/>
+      <c r="H139" s="12"/>
+      <c r="I139" s="12"/>
+      <c r="J139" s="13"/>
       <c r="K139" s="10"/>
     </row>
     <row r="140" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A140" s="12"/>
-      <c r="B140" s="12"/>
+      <c r="A140" s="11"/>
+      <c r="B140" s="11"/>
       <c r="C140" s="10"/>
-      <c r="D140" s="12"/>
+      <c r="D140" s="11"/>
       <c r="E140" s="0"/>
-      <c r="F140" s="12"/>
-      <c r="G140" s="12"/>
-      <c r="H140" s="13"/>
-      <c r="I140" s="13"/>
-      <c r="J140" s="14"/>
+      <c r="F140" s="11"/>
+      <c r="G140" s="11"/>
+      <c r="H140" s="12"/>
+      <c r="I140" s="12"/>
+      <c r="J140" s="13"/>
       <c r="K140" s="10"/>
     </row>
     <row r="141" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A141" s="12"/>
-      <c r="B141" s="12"/>
+      <c r="A141" s="11"/>
+      <c r="B141" s="11"/>
       <c r="C141" s="10"/>
-      <c r="D141" s="12"/>
+      <c r="D141" s="11"/>
       <c r="E141" s="0"/>
-      <c r="F141" s="12"/>
-      <c r="G141" s="12"/>
-      <c r="H141" s="13"/>
-      <c r="I141" s="13"/>
-      <c r="J141" s="14"/>
+      <c r="F141" s="11"/>
+      <c r="G141" s="11"/>
+      <c r="H141" s="12"/>
+      <c r="I141" s="12"/>
+      <c r="J141" s="13"/>
       <c r="K141" s="10"/>
     </row>
     <row r="142" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A142" s="12"/>
-      <c r="B142" s="12"/>
+      <c r="A142" s="11"/>
+      <c r="B142" s="11"/>
       <c r="C142" s="10"/>
-      <c r="D142" s="12"/>
+      <c r="D142" s="11"/>
       <c r="E142" s="4"/>
-      <c r="F142" s="12"/>
-      <c r="G142" s="12"/>
-      <c r="H142" s="13"/>
-      <c r="I142" s="13"/>
-      <c r="J142" s="14"/>
+      <c r="F142" s="11"/>
+      <c r="G142" s="11"/>
+      <c r="H142" s="12"/>
+      <c r="I142" s="12"/>
+      <c r="J142" s="13"/>
       <c r="K142" s="10"/>
     </row>
   </sheetData>

</xml_diff>